<commit_message>
4th commit where the business logic which actually allocates the parking spots based on date of joining has been implemented
</commit_message>
<xml_diff>
--- a/ssa-carpark/src/main/resources/employee_parking_details.xlsx
+++ b/ssa-carpark/src/main/resources/employee_parking_details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="ssa_employees" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="40">
   <si>
     <t>Employee Id</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>Employee Email Address</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>SG Fleet Customer</t>
+  </si>
+  <si>
+    <t>PM Partners</t>
+  </si>
+  <si>
+    <t>Fleet Partners</t>
   </si>
 </sst>
 </file>
@@ -518,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +635,7 @@
         <v>38404</v>
       </c>
       <c r="D4" s="2">
-        <v>42684</v>
+        <v>42679</v>
       </c>
       <c r="E4" s="2">
         <v>42694</v>
@@ -834,10 +846,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +860,7 @@
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -858,8 +870,11 @@
       <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>8</v>
       </c>
@@ -869,8 +884,11 @@
       <c r="C2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>173</v>
       </c>
@@ -880,8 +898,11 @@
       <c r="C3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
@@ -891,8 +912,11 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>175</v>
       </c>
@@ -902,8 +926,11 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7</v>
       </c>
@@ -913,8 +940,11 @@
       <c r="C6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>176</v>
       </c>
@@ -924,8 +954,11 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>177</v>
       </c>
@@ -935,8 +968,11 @@
       <c r="C8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>178</v>
       </c>
@@ -946,8 +982,11 @@
       <c r="C9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>179</v>
       </c>
@@ -956,6 +995,9 @@
       </c>
       <c r="C10" t="s">
         <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>